<commit_message>
Replacing the accession names coded with "-" to "_" in order to match the genotype names specified in the genetic maps.
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/DerivedData/AccessionMap.xlsx
+++ b/Data/phenotypic data/DerivedData/AccessionMap.xlsx
@@ -21,114 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="257">
   <si>
-    <t>CNJ04-2-1</t>
-  </si>
-  <si>
-    <t>CNJ04-2-2</t>
-  </si>
-  <si>
-    <t>CNJ04-2-3</t>
-  </si>
-  <si>
-    <t>CNJ04-2-4</t>
-  </si>
-  <si>
-    <t>CNJ04-2-5</t>
-  </si>
-  <si>
-    <t>CNJ04-2-6</t>
-  </si>
-  <si>
-    <t>CNJ04-2-7</t>
-  </si>
-  <si>
-    <t>CNJ04-2-8</t>
-  </si>
-  <si>
-    <t>CNJ04-2-9</t>
-  </si>
-  <si>
-    <t>CNJ04-2-10</t>
-  </si>
-  <si>
-    <t>CNJ04-2-11</t>
-  </si>
-  <si>
-    <t>CNJ04-2-12</t>
-  </si>
-  <si>
-    <t>CNJ04-2-13</t>
-  </si>
-  <si>
-    <t>CNJ04-2-14</t>
-  </si>
-  <si>
-    <t>CNJ04-2-15</t>
-  </si>
-  <si>
-    <t>CNJ04-2-16</t>
-  </si>
-  <si>
-    <t>CNJ04-2-17</t>
-  </si>
-  <si>
-    <t>CNJ04-2-18</t>
-  </si>
-  <si>
-    <t>CNJ04-2-19</t>
-  </si>
-  <si>
-    <t>CNJ04-2-20</t>
-  </si>
-  <si>
-    <t>CNJ04-2-21</t>
-  </si>
-  <si>
-    <t>CNJ04-2-22</t>
-  </si>
-  <si>
-    <t>CNJ04-2-23</t>
-  </si>
-  <si>
-    <t>CNJ04-2-24</t>
-  </si>
-  <si>
-    <t>CNJ04-2-25</t>
-  </si>
-  <si>
-    <t>CNJ04-2-26</t>
-  </si>
-  <si>
-    <t>CNJ04-2-27</t>
-  </si>
-  <si>
-    <t>CNJ04-2-28</t>
-  </si>
-  <si>
-    <t>CNJ04-2-29</t>
-  </si>
-  <si>
-    <t>CNJ04-2-30</t>
-  </si>
-  <si>
-    <t>CNJ04-2-31</t>
-  </si>
-  <si>
-    <t>CNJ04-2-32</t>
-  </si>
-  <si>
-    <t>CNJ04-2-33</t>
-  </si>
-  <si>
-    <t>CNJ04-2-34</t>
-  </si>
-  <si>
-    <t>CNJ04-2-35</t>
-  </si>
-  <si>
-    <t>CNJ04-2-36</t>
-  </si>
-  <si>
     <t>Row</t>
   </si>
   <si>
@@ -138,658 +30,766 @@
     <t>NJ Accession</t>
   </si>
   <si>
-    <t>CNJ04-21-1</t>
-  </si>
-  <si>
-    <t>CNJ04-21-2</t>
-  </si>
-  <si>
-    <t>CNJ04-21-3</t>
-  </si>
-  <si>
-    <t>CNJ04-21-4</t>
-  </si>
-  <si>
-    <t>CNJ04-21-5</t>
-  </si>
-  <si>
-    <t>CNJ04-21-6</t>
-  </si>
-  <si>
-    <t>CNJ04-21-7</t>
-  </si>
-  <si>
-    <t>CNJ04-21-8</t>
-  </si>
-  <si>
-    <t>CNJ04-21-9</t>
-  </si>
-  <si>
-    <t>CNJ04-21-10</t>
-  </si>
-  <si>
-    <t>CNJ04-21-11</t>
-  </si>
-  <si>
-    <t>CNJ04-21-12</t>
-  </si>
-  <si>
-    <t>CNJ04-21-13</t>
-  </si>
-  <si>
-    <t>CNJ04-21-14</t>
-  </si>
-  <si>
-    <t>CNJ04-21-15</t>
-  </si>
-  <si>
-    <t>CNJ04-21-16</t>
-  </si>
-  <si>
-    <t>CNJ04-21-17</t>
-  </si>
-  <si>
-    <t>CNJ04-21-18</t>
-  </si>
-  <si>
-    <t>CNJ04-21-19</t>
-  </si>
-  <si>
-    <t>CNJ04-21-20</t>
-  </si>
-  <si>
-    <t>CNJ04-21-21</t>
-  </si>
-  <si>
-    <t>CNJ04-21-22</t>
-  </si>
-  <si>
-    <t>CNJ04-21-23</t>
-  </si>
-  <si>
-    <t>CNJ04-21-24</t>
-  </si>
-  <si>
-    <t>CNJ04-21-25</t>
-  </si>
-  <si>
-    <t>CNJ04-21-26</t>
-  </si>
-  <si>
-    <t>CNJ04-21-27</t>
-  </si>
-  <si>
-    <t>CNJ04-21-28</t>
-  </si>
-  <si>
-    <t>CNJ04-21-29</t>
-  </si>
-  <si>
-    <t>CNJ04-21-30</t>
-  </si>
-  <si>
-    <t>CNJ04-21-31</t>
-  </si>
-  <si>
-    <t>CNJ04-21-32</t>
-  </si>
-  <si>
-    <t>CNJ04-21-33</t>
-  </si>
-  <si>
-    <t>CNJ04-21-34</t>
-  </si>
-  <si>
-    <t>CNJ04-21-35</t>
-  </si>
-  <si>
-    <t>CNJ04-21-36</t>
-  </si>
-  <si>
     <t>Stevens</t>
   </si>
   <si>
     <t>Mullica Queen</t>
   </si>
   <si>
-    <t>CNJ02-1-1</t>
-  </si>
-  <si>
-    <t>CNJ02-1-2</t>
-  </si>
-  <si>
-    <t>CNJ02-1-3</t>
-  </si>
-  <si>
-    <t>CNJ02-1-4</t>
-  </si>
-  <si>
-    <t>CNJ02-1-5</t>
-  </si>
-  <si>
-    <t>CNJ02-1-6</t>
-  </si>
-  <si>
-    <t>CNJ02-1-7</t>
-  </si>
-  <si>
-    <t>CNJ02-1-8</t>
-  </si>
-  <si>
-    <t>CNJ02-1-9</t>
-  </si>
-  <si>
-    <t>CNJ02-1-10</t>
-  </si>
-  <si>
-    <t>CNJ02-1-11</t>
-  </si>
-  <si>
-    <t>CNJ02-1-12</t>
-  </si>
-  <si>
-    <t>CNJ02-1-13</t>
-  </si>
-  <si>
-    <t>CNJ02-1-14</t>
-  </si>
-  <si>
-    <t>CNJ02-1-15</t>
-  </si>
-  <si>
-    <t>CNJ02-1-16</t>
-  </si>
-  <si>
-    <t>CNJ02-1-17</t>
-  </si>
-  <si>
-    <t>CNJ02-1-18</t>
-  </si>
-  <si>
-    <t>CNJ02-1-19</t>
-  </si>
-  <si>
-    <t>CNJ02-1-20</t>
-  </si>
-  <si>
-    <t>CNJ02-1-21</t>
-  </si>
-  <si>
-    <t>CNJ02-1-22</t>
-  </si>
-  <si>
-    <t>CNJ02-1-23</t>
-  </si>
-  <si>
-    <t>CNJ02-1-24</t>
-  </si>
-  <si>
-    <t>CNJ02-1-25</t>
-  </si>
-  <si>
-    <t>CNJ02-1-26</t>
-  </si>
-  <si>
-    <t>CNJ02-1-27</t>
-  </si>
-  <si>
-    <t>CNJ02-1-28</t>
-  </si>
-  <si>
-    <t>CNJ02-1-29</t>
-  </si>
-  <si>
-    <t>CNJ02-1-30</t>
-  </si>
-  <si>
-    <t>CNJ02-1-31</t>
-  </si>
-  <si>
-    <t>CNJ02-1-32</t>
-  </si>
-  <si>
-    <t>CNJ02-1-33</t>
-  </si>
-  <si>
-    <t>CNJ02-1-34</t>
-  </si>
-  <si>
-    <t>CNJ02-1-35</t>
-  </si>
-  <si>
-    <t>CNJ02-1-36</t>
-  </si>
-  <si>
-    <t>CNJ02-1-37</t>
-  </si>
-  <si>
-    <t>CNJ02-1-38</t>
-  </si>
-  <si>
-    <t>CNJ02-1-39</t>
-  </si>
-  <si>
-    <t>CNJ02-1-40</t>
-  </si>
-  <si>
-    <t>CNJ02-1-41</t>
-  </si>
-  <si>
-    <t>CNJ02-1-42</t>
-  </si>
-  <si>
-    <t>CNJ02-1-43</t>
-  </si>
-  <si>
-    <t>CNJ02-1-44</t>
-  </si>
-  <si>
-    <t>CNJ02-1-45</t>
-  </si>
-  <si>
-    <t>CNJ02-1-46</t>
-  </si>
-  <si>
-    <t>CNJ02-1-47</t>
-  </si>
-  <si>
-    <t>CNJ02-1-48</t>
-  </si>
-  <si>
-    <t>CNJ02-1-49</t>
-  </si>
-  <si>
-    <t>CNJ02-1-50</t>
-  </si>
-  <si>
-    <t>CNJ02-1-51</t>
-  </si>
-  <si>
-    <t>CNJ02-1-52</t>
-  </si>
-  <si>
-    <t>CNJ02-1-53</t>
-  </si>
-  <si>
-    <t>CNJ02-1-54</t>
-  </si>
-  <si>
-    <t>CNJ02-1-55</t>
-  </si>
-  <si>
-    <t>CNJ02-1-56</t>
-  </si>
-  <si>
-    <t>CNJ02-1-57</t>
-  </si>
-  <si>
-    <t>CNJ02-1-58</t>
-  </si>
-  <si>
-    <t>CNJ02-1-59</t>
-  </si>
-  <si>
-    <t>CNJ02-1-60</t>
-  </si>
-  <si>
-    <t>CNJ02-1-61</t>
-  </si>
-  <si>
-    <t>CNJ02-1-62</t>
-  </si>
-  <si>
-    <t>CNJ02-1-63</t>
-  </si>
-  <si>
-    <t>CNJ02-1-64</t>
-  </si>
-  <si>
-    <t>CNJ02-1-65</t>
-  </si>
-  <si>
-    <t>CNJ02-1-66</t>
-  </si>
-  <si>
-    <t>CNJ02-1-67</t>
-  </si>
-  <si>
-    <t>CNJ02-1-68</t>
-  </si>
-  <si>
-    <t>CNJ02-1-69</t>
-  </si>
-  <si>
-    <t>CNJ02-1-70</t>
-  </si>
-  <si>
-    <t>CNJ02-1-71</t>
-  </si>
-  <si>
-    <t>CNJ02-1-72</t>
-  </si>
-  <si>
-    <t>CNJ02-1-73</t>
-  </si>
-  <si>
-    <t>CNJ02-1-74</t>
-  </si>
-  <si>
-    <t>CNJ02-1-75</t>
-  </si>
-  <si>
-    <t>CNJ02-1-76</t>
-  </si>
-  <si>
-    <t>CNJ02-1-77</t>
-  </si>
-  <si>
-    <t>CNJ02-1-78</t>
-  </si>
-  <si>
-    <t>CNJ02-1-79</t>
-  </si>
-  <si>
-    <t>CNJ02-1-80</t>
-  </si>
-  <si>
-    <t>CNJ02-1-81</t>
-  </si>
-  <si>
-    <t>CNJ02-1-82</t>
-  </si>
-  <si>
-    <t>CNJ02-1-83</t>
-  </si>
-  <si>
-    <t>CNJ02-1-84</t>
-  </si>
-  <si>
-    <t>CNJ02-1-85</t>
-  </si>
-  <si>
-    <t>CNJ02-1-86</t>
-  </si>
-  <si>
-    <t>CNJ02-1-87</t>
-  </si>
-  <si>
-    <t>CNJ02-1-88</t>
-  </si>
-  <si>
-    <t>CNJ02-1-89</t>
-  </si>
-  <si>
-    <t>CNJ02-1-90</t>
-  </si>
-  <si>
-    <t>CNJ02-1-91</t>
-  </si>
-  <si>
-    <t>CNJ02-1-92</t>
-  </si>
-  <si>
-    <t>CNJ02-1-93</t>
-  </si>
-  <si>
-    <t>CNJ02-1-94</t>
-  </si>
-  <si>
-    <t>CNJ02-1-95</t>
-  </si>
-  <si>
-    <t>CNJ02-1-96</t>
-  </si>
-  <si>
-    <t>CNJ02-1-97</t>
-  </si>
-  <si>
-    <t>CNJ02-1-98</t>
-  </si>
-  <si>
-    <t>CNJ02-1-99</t>
-  </si>
-  <si>
-    <t>CNJ02-1-100</t>
-  </si>
-  <si>
-    <t>CNJ02-1-101</t>
-  </si>
-  <si>
-    <t>CNJ02-1-102</t>
-  </si>
-  <si>
-    <t>CNJ02-1-103</t>
-  </si>
-  <si>
-    <t>CNJ02-1-104</t>
-  </si>
-  <si>
-    <t>CNJ02-1-105</t>
-  </si>
-  <si>
-    <t>CNJ02-1-106</t>
-  </si>
-  <si>
-    <t>CNJ02-1-107</t>
-  </si>
-  <si>
-    <t>CNJ02-1-108</t>
-  </si>
-  <si>
-    <t>CNJ02-1-109</t>
-  </si>
-  <si>
-    <t>CNJ02-1-110</t>
-  </si>
-  <si>
-    <t>CNJ02-1-111</t>
-  </si>
-  <si>
-    <t>CNJ02-1-112</t>
-  </si>
-  <si>
-    <t>CNJ02-1-113</t>
-  </si>
-  <si>
-    <t>CNJ02-1-114</t>
-  </si>
-  <si>
-    <t>CNJ02-1-115</t>
-  </si>
-  <si>
-    <t>CNJ02-1-116</t>
-  </si>
-  <si>
-    <t>CNJ02-1-117</t>
-  </si>
-  <si>
-    <t>CNJ02-1-118</t>
-  </si>
-  <si>
-    <t>CNJ02-1-119</t>
-  </si>
-  <si>
-    <t>CNJ02-1-120</t>
-  </si>
-  <si>
-    <t>CNJ02-1-121</t>
-  </si>
-  <si>
-    <t>CNJ02-1-122</t>
-  </si>
-  <si>
-    <t>CNJ02-1-123</t>
-  </si>
-  <si>
-    <t>CNJ02-1-124</t>
-  </si>
-  <si>
-    <t>CNJ02-1-125</t>
-  </si>
-  <si>
-    <t>CNJ02-1-126</t>
-  </si>
-  <si>
-    <t>CNJ02-1-127</t>
-  </si>
-  <si>
-    <t>CNJ02-1-128</t>
-  </si>
-  <si>
-    <t>CNJ02-1-129</t>
-  </si>
-  <si>
-    <t>CNJ02-1-130</t>
-  </si>
-  <si>
-    <t>CNJ02-1-131</t>
-  </si>
-  <si>
-    <t>CNJ02-1-132</t>
-  </si>
-  <si>
-    <t>CNJ02-1-133</t>
-  </si>
-  <si>
-    <t>CNJ02-1-134</t>
-  </si>
-  <si>
-    <t>CNJ02-1-135</t>
-  </si>
-  <si>
-    <t>CNJ02-1-136</t>
-  </si>
-  <si>
-    <t>CNJ02-1-137</t>
-  </si>
-  <si>
-    <t>CNJ02-1-138</t>
-  </si>
-  <si>
-    <t>CNJ02-1-139</t>
-  </si>
-  <si>
-    <t>CNJ02-1-140</t>
-  </si>
-  <si>
-    <t>CNJ02-1-141</t>
-  </si>
-  <si>
-    <t>CNJ02-1-142</t>
-  </si>
-  <si>
-    <t>CNJ02-1-143</t>
-  </si>
-  <si>
-    <t>CNJ02-1-144</t>
-  </si>
-  <si>
-    <t>CNJ02-1-145</t>
-  </si>
-  <si>
-    <t>CNJ02-1-146</t>
-  </si>
-  <si>
-    <t>CNJ02-1-147</t>
-  </si>
-  <si>
-    <t>CNJ02-1-148</t>
-  </si>
-  <si>
-    <t>CNJ02-1-149</t>
-  </si>
-  <si>
-    <t>CNJ02-1-150</t>
-  </si>
-  <si>
-    <t>CNJ02-1-151</t>
-  </si>
-  <si>
-    <t>CNJ02-1-152</t>
-  </si>
-  <si>
-    <t>CNJ02-1-153</t>
-  </si>
-  <si>
-    <t>CNJ02-1-154</t>
-  </si>
-  <si>
-    <t>CNJ02-1-155</t>
-  </si>
-  <si>
-    <t>CNJ02-1-156</t>
-  </si>
-  <si>
-    <t>CNJ02-1-157</t>
-  </si>
-  <si>
-    <t>CNJ02-1-167</t>
-  </si>
-  <si>
-    <t>CNJ02-1-171</t>
-  </si>
-  <si>
-    <t>CNJ02-1-172</t>
-  </si>
-  <si>
-    <t>CNJ02-1-177</t>
-  </si>
-  <si>
-    <t>CNJ02-1-181</t>
-  </si>
-  <si>
-    <t>CNJ02-1-182</t>
-  </si>
-  <si>
-    <t>CNJ02-1-186</t>
-  </si>
-  <si>
-    <t>CNJ02-1-187</t>
-  </si>
-  <si>
-    <t>CNJ02-1-188</t>
-  </si>
-  <si>
-    <t>CNJ02-1-189</t>
-  </si>
-  <si>
-    <t>CNJ02-1-191</t>
-  </si>
-  <si>
-    <t>CNJ02-1-193</t>
-  </si>
-  <si>
-    <t>CNJ02-1-198</t>
-  </si>
-  <si>
-    <t>CNJ02-1-200</t>
-  </si>
-  <si>
-    <t>CNJ02-1-201</t>
-  </si>
-  <si>
-    <t>CNJ02-1-203</t>
-  </si>
-  <si>
-    <t>CNJ02-1-204</t>
-  </si>
-  <si>
-    <t>CNJ02-1-207</t>
-  </si>
-  <si>
-    <t>CNJ02-1-225</t>
-  </si>
-  <si>
-    <t>CNJ02-1-226</t>
-  </si>
-  <si>
-    <t>CNJ02-1-228</t>
-  </si>
-  <si>
-    <t>CNJ02-1-235</t>
-  </si>
-  <si>
     <t>Crimson Queen</t>
+  </si>
+  <si>
+    <t>CNJ04_2_1</t>
+  </si>
+  <si>
+    <t>CNJ04_2_2</t>
+  </si>
+  <si>
+    <t>CNJ04_2_3</t>
+  </si>
+  <si>
+    <t>CNJ04_2_4</t>
+  </si>
+  <si>
+    <t>CNJ04_2_5</t>
+  </si>
+  <si>
+    <t>CNJ04_2_6</t>
+  </si>
+  <si>
+    <t>CNJ04_2_7</t>
+  </si>
+  <si>
+    <t>CNJ04_2_8</t>
+  </si>
+  <si>
+    <t>CNJ04_2_9</t>
+  </si>
+  <si>
+    <t>CNJ04_2_10</t>
+  </si>
+  <si>
+    <t>CNJ04_2_11</t>
+  </si>
+  <si>
+    <t>CNJ04_2_12</t>
+  </si>
+  <si>
+    <t>CNJ04_2_13</t>
+  </si>
+  <si>
+    <t>CNJ04_2_14</t>
+  </si>
+  <si>
+    <t>CNJ04_2_15</t>
+  </si>
+  <si>
+    <t>CNJ04_2_16</t>
+  </si>
+  <si>
+    <t>CNJ04_2_17</t>
+  </si>
+  <si>
+    <t>CNJ04_2_18</t>
+  </si>
+  <si>
+    <t>CNJ04_2_19</t>
+  </si>
+  <si>
+    <t>CNJ04_2_20</t>
+  </si>
+  <si>
+    <t>CNJ04_2_21</t>
+  </si>
+  <si>
+    <t>CNJ04_2_22</t>
+  </si>
+  <si>
+    <t>CNJ04_2_23</t>
+  </si>
+  <si>
+    <t>CNJ04_2_24</t>
+  </si>
+  <si>
+    <t>CNJ04_2_25</t>
+  </si>
+  <si>
+    <t>CNJ04_2_26</t>
+  </si>
+  <si>
+    <t>CNJ04_2_27</t>
+  </si>
+  <si>
+    <t>CNJ04_2_28</t>
+  </si>
+  <si>
+    <t>CNJ04_2_29</t>
+  </si>
+  <si>
+    <t>CNJ04_2_30</t>
+  </si>
+  <si>
+    <t>CNJ04_2_31</t>
+  </si>
+  <si>
+    <t>CNJ04_2_32</t>
+  </si>
+  <si>
+    <t>CNJ04_2_33</t>
+  </si>
+  <si>
+    <t>CNJ04_2_34</t>
+  </si>
+  <si>
+    <t>CNJ04_2_35</t>
+  </si>
+  <si>
+    <t>CNJ04_2_36</t>
+  </si>
+  <si>
+    <t>CNJ04_21_1</t>
+  </si>
+  <si>
+    <t>CNJ04_21_2</t>
+  </si>
+  <si>
+    <t>CNJ04_21_3</t>
+  </si>
+  <si>
+    <t>CNJ04_21_4</t>
+  </si>
+  <si>
+    <t>CNJ04_21_5</t>
+  </si>
+  <si>
+    <t>CNJ04_21_6</t>
+  </si>
+  <si>
+    <t>CNJ04_21_7</t>
+  </si>
+  <si>
+    <t>CNJ04_21_8</t>
+  </si>
+  <si>
+    <t>CNJ04_21_9</t>
+  </si>
+  <si>
+    <t>CNJ04_21_10</t>
+  </si>
+  <si>
+    <t>CNJ04_21_11</t>
+  </si>
+  <si>
+    <t>CNJ04_21_12</t>
+  </si>
+  <si>
+    <t>CNJ04_21_13</t>
+  </si>
+  <si>
+    <t>CNJ04_21_14</t>
+  </si>
+  <si>
+    <t>CNJ04_21_15</t>
+  </si>
+  <si>
+    <t>CNJ04_21_16</t>
+  </si>
+  <si>
+    <t>CNJ04_21_17</t>
+  </si>
+  <si>
+    <t>CNJ04_21_18</t>
+  </si>
+  <si>
+    <t>CNJ04_21_19</t>
+  </si>
+  <si>
+    <t>CNJ04_21_20</t>
+  </si>
+  <si>
+    <t>CNJ04_21_21</t>
+  </si>
+  <si>
+    <t>CNJ04_21_22</t>
+  </si>
+  <si>
+    <t>CNJ04_21_23</t>
+  </si>
+  <si>
+    <t>CNJ04_21_24</t>
+  </si>
+  <si>
+    <t>CNJ04_21_25</t>
+  </si>
+  <si>
+    <t>CNJ04_21_26</t>
+  </si>
+  <si>
+    <t>CNJ04_21_27</t>
+  </si>
+  <si>
+    <t>CNJ04_21_28</t>
+  </si>
+  <si>
+    <t>CNJ04_21_29</t>
+  </si>
+  <si>
+    <t>CNJ04_21_30</t>
+  </si>
+  <si>
+    <t>CNJ04_21_31</t>
+  </si>
+  <si>
+    <t>CNJ04_21_32</t>
+  </si>
+  <si>
+    <t>CNJ04_21_33</t>
+  </si>
+  <si>
+    <t>CNJ04_21_34</t>
+  </si>
+  <si>
+    <t>CNJ04_21_35</t>
+  </si>
+  <si>
+    <t>CNJ04_21_36</t>
+  </si>
+  <si>
+    <t>CNJ02_1_1</t>
+  </si>
+  <si>
+    <t>CNJ02_1_2</t>
+  </si>
+  <si>
+    <t>CNJ02_1_3</t>
+  </si>
+  <si>
+    <t>CNJ02_1_4</t>
+  </si>
+  <si>
+    <t>CNJ02_1_5</t>
+  </si>
+  <si>
+    <t>CNJ02_1_6</t>
+  </si>
+  <si>
+    <t>CNJ02_1_7</t>
+  </si>
+  <si>
+    <t>CNJ02_1_8</t>
+  </si>
+  <si>
+    <t>CNJ02_1_9</t>
+  </si>
+  <si>
+    <t>CNJ02_1_10</t>
+  </si>
+  <si>
+    <t>CNJ02_1_11</t>
+  </si>
+  <si>
+    <t>CNJ02_1_12</t>
+  </si>
+  <si>
+    <t>CNJ02_1_13</t>
+  </si>
+  <si>
+    <t>CNJ02_1_14</t>
+  </si>
+  <si>
+    <t>CNJ02_1_15</t>
+  </si>
+  <si>
+    <t>CNJ02_1_16</t>
+  </si>
+  <si>
+    <t>CNJ02_1_17</t>
+  </si>
+  <si>
+    <t>CNJ02_1_18</t>
+  </si>
+  <si>
+    <t>CNJ02_1_19</t>
+  </si>
+  <si>
+    <t>CNJ02_1_20</t>
+  </si>
+  <si>
+    <t>CNJ02_1_21</t>
+  </si>
+  <si>
+    <t>CNJ02_1_22</t>
+  </si>
+  <si>
+    <t>CNJ02_1_23</t>
+  </si>
+  <si>
+    <t>CNJ02_1_24</t>
+  </si>
+  <si>
+    <t>CNJ02_1_25</t>
+  </si>
+  <si>
+    <t>CNJ02_1_26</t>
+  </si>
+  <si>
+    <t>CNJ02_1_27</t>
+  </si>
+  <si>
+    <t>CNJ02_1_28</t>
+  </si>
+  <si>
+    <t>CNJ02_1_29</t>
+  </si>
+  <si>
+    <t>CNJ02_1_30</t>
+  </si>
+  <si>
+    <t>CNJ02_1_31</t>
+  </si>
+  <si>
+    <t>CNJ02_1_32</t>
+  </si>
+  <si>
+    <t>CNJ02_1_33</t>
+  </si>
+  <si>
+    <t>CNJ02_1_34</t>
+  </si>
+  <si>
+    <t>CNJ02_1_35</t>
+  </si>
+  <si>
+    <t>CNJ02_1_36</t>
+  </si>
+  <si>
+    <t>CNJ02_1_37</t>
+  </si>
+  <si>
+    <t>CNJ02_1_38</t>
+  </si>
+  <si>
+    <t>CNJ02_1_39</t>
+  </si>
+  <si>
+    <t>CNJ02_1_40</t>
+  </si>
+  <si>
+    <t>CNJ02_1_41</t>
+  </si>
+  <si>
+    <t>CNJ02_1_42</t>
+  </si>
+  <si>
+    <t>CNJ02_1_43</t>
+  </si>
+  <si>
+    <t>CNJ02_1_44</t>
+  </si>
+  <si>
+    <t>CNJ02_1_45</t>
+  </si>
+  <si>
+    <t>CNJ02_1_46</t>
+  </si>
+  <si>
+    <t>CNJ02_1_47</t>
+  </si>
+  <si>
+    <t>CNJ02_1_48</t>
+  </si>
+  <si>
+    <t>CNJ02_1_49</t>
+  </si>
+  <si>
+    <t>CNJ02_1_50</t>
+  </si>
+  <si>
+    <t>CNJ02_1_51</t>
+  </si>
+  <si>
+    <t>CNJ02_1_52</t>
+  </si>
+  <si>
+    <t>CNJ02_1_53</t>
+  </si>
+  <si>
+    <t>CNJ02_1_54</t>
+  </si>
+  <si>
+    <t>CNJ02_1_55</t>
+  </si>
+  <si>
+    <t>CNJ02_1_56</t>
+  </si>
+  <si>
+    <t>CNJ02_1_57</t>
+  </si>
+  <si>
+    <t>CNJ02_1_58</t>
+  </si>
+  <si>
+    <t>CNJ02_1_59</t>
+  </si>
+  <si>
+    <t>CNJ02_1_60</t>
+  </si>
+  <si>
+    <t>CNJ02_1_61</t>
+  </si>
+  <si>
+    <t>CNJ02_1_62</t>
+  </si>
+  <si>
+    <t>CNJ02_1_63</t>
+  </si>
+  <si>
+    <t>CNJ02_1_64</t>
+  </si>
+  <si>
+    <t>CNJ02_1_65</t>
+  </si>
+  <si>
+    <t>CNJ02_1_66</t>
+  </si>
+  <si>
+    <t>CNJ02_1_67</t>
+  </si>
+  <si>
+    <t>CNJ02_1_68</t>
+  </si>
+  <si>
+    <t>CNJ02_1_69</t>
+  </si>
+  <si>
+    <t>CNJ02_1_70</t>
+  </si>
+  <si>
+    <t>CNJ02_1_71</t>
+  </si>
+  <si>
+    <t>CNJ02_1_72</t>
+  </si>
+  <si>
+    <t>CNJ02_1_73</t>
+  </si>
+  <si>
+    <t>CNJ02_1_74</t>
+  </si>
+  <si>
+    <t>CNJ02_1_75</t>
+  </si>
+  <si>
+    <t>CNJ02_1_76</t>
+  </si>
+  <si>
+    <t>CNJ02_1_77</t>
+  </si>
+  <si>
+    <t>CNJ02_1_78</t>
+  </si>
+  <si>
+    <t>CNJ02_1_79</t>
+  </si>
+  <si>
+    <t>CNJ02_1_80</t>
+  </si>
+  <si>
+    <t>CNJ02_1_81</t>
+  </si>
+  <si>
+    <t>CNJ02_1_82</t>
+  </si>
+  <si>
+    <t>CNJ02_1_83</t>
+  </si>
+  <si>
+    <t>CNJ02_1_84</t>
+  </si>
+  <si>
+    <t>CNJ02_1_85</t>
+  </si>
+  <si>
+    <t>CNJ02_1_86</t>
+  </si>
+  <si>
+    <t>CNJ02_1_87</t>
+  </si>
+  <si>
+    <t>CNJ02_1_88</t>
+  </si>
+  <si>
+    <t>CNJ02_1_89</t>
+  </si>
+  <si>
+    <t>CNJ02_1_90</t>
+  </si>
+  <si>
+    <t>CNJ02_1_91</t>
+  </si>
+  <si>
+    <t>CNJ02_1_92</t>
+  </si>
+  <si>
+    <t>CNJ02_1_93</t>
+  </si>
+  <si>
+    <t>CNJ02_1_94</t>
+  </si>
+  <si>
+    <t>CNJ02_1_95</t>
+  </si>
+  <si>
+    <t>CNJ02_1_96</t>
+  </si>
+  <si>
+    <t>CNJ02_1_97</t>
+  </si>
+  <si>
+    <t>CNJ02_1_98</t>
+  </si>
+  <si>
+    <t>CNJ02_1_99</t>
+  </si>
+  <si>
+    <t>CNJ02_1_100</t>
+  </si>
+  <si>
+    <t>CNJ02_1_101</t>
+  </si>
+  <si>
+    <t>CNJ02_1_102</t>
+  </si>
+  <si>
+    <t>CNJ02_1_103</t>
+  </si>
+  <si>
+    <t>CNJ02_1_104</t>
+  </si>
+  <si>
+    <t>CNJ02_1_105</t>
+  </si>
+  <si>
+    <t>CNJ02_1_106</t>
+  </si>
+  <si>
+    <t>CNJ02_1_107</t>
+  </si>
+  <si>
+    <t>CNJ02_1_108</t>
+  </si>
+  <si>
+    <t>CNJ02_1_109</t>
+  </si>
+  <si>
+    <t>CNJ02_1_110</t>
+  </si>
+  <si>
+    <t>CNJ02_1_111</t>
+  </si>
+  <si>
+    <t>CNJ02_1_112</t>
+  </si>
+  <si>
+    <t>CNJ02_1_113</t>
+  </si>
+  <si>
+    <t>CNJ02_1_114</t>
+  </si>
+  <si>
+    <t>CNJ02_1_115</t>
+  </si>
+  <si>
+    <t>CNJ02_1_116</t>
+  </si>
+  <si>
+    <t>CNJ02_1_117</t>
+  </si>
+  <si>
+    <t>CNJ02_1_118</t>
+  </si>
+  <si>
+    <t>CNJ02_1_119</t>
+  </si>
+  <si>
+    <t>CNJ02_1_120</t>
+  </si>
+  <si>
+    <t>CNJ02_1_121</t>
+  </si>
+  <si>
+    <t>CNJ02_1_122</t>
+  </si>
+  <si>
+    <t>CNJ02_1_123</t>
+  </si>
+  <si>
+    <t>CNJ02_1_124</t>
+  </si>
+  <si>
+    <t>CNJ02_1_125</t>
+  </si>
+  <si>
+    <t>CNJ02_1_126</t>
+  </si>
+  <si>
+    <t>CNJ02_1_127</t>
+  </si>
+  <si>
+    <t>CNJ02_1_128</t>
+  </si>
+  <si>
+    <t>CNJ02_1_129</t>
+  </si>
+  <si>
+    <t>CNJ02_1_130</t>
+  </si>
+  <si>
+    <t>CNJ02_1_131</t>
+  </si>
+  <si>
+    <t>CNJ02_1_132</t>
+  </si>
+  <si>
+    <t>CNJ02_1_133</t>
+  </si>
+  <si>
+    <t>CNJ02_1_134</t>
+  </si>
+  <si>
+    <t>CNJ02_1_135</t>
+  </si>
+  <si>
+    <t>CNJ02_1_136</t>
+  </si>
+  <si>
+    <t>CNJ02_1_137</t>
+  </si>
+  <si>
+    <t>CNJ02_1_138</t>
+  </si>
+  <si>
+    <t>CNJ02_1_139</t>
+  </si>
+  <si>
+    <t>CNJ02_1_140</t>
+  </si>
+  <si>
+    <t>CNJ02_1_141</t>
+  </si>
+  <si>
+    <t>CNJ02_1_142</t>
+  </si>
+  <si>
+    <t>CNJ02_1_143</t>
+  </si>
+  <si>
+    <t>CNJ02_1_144</t>
+  </si>
+  <si>
+    <t>CNJ02_1_145</t>
+  </si>
+  <si>
+    <t>CNJ02_1_146</t>
+  </si>
+  <si>
+    <t>CNJ02_1_147</t>
+  </si>
+  <si>
+    <t>CNJ02_1_148</t>
+  </si>
+  <si>
+    <t>CNJ02_1_149</t>
+  </si>
+  <si>
+    <t>CNJ02_1_150</t>
+  </si>
+  <si>
+    <t>CNJ02_1_151</t>
+  </si>
+  <si>
+    <t>CNJ02_1_152</t>
+  </si>
+  <si>
+    <t>CNJ02_1_153</t>
+  </si>
+  <si>
+    <t>CNJ02_1_154</t>
+  </si>
+  <si>
+    <t>CNJ02_1_155</t>
+  </si>
+  <si>
+    <t>CNJ02_1_156</t>
+  </si>
+  <si>
+    <t>CNJ02_1_157</t>
+  </si>
+  <si>
+    <t>CNJ02_1_167</t>
+  </si>
+  <si>
+    <t>CNJ02_1_171</t>
+  </si>
+  <si>
+    <t>CNJ02_1_172</t>
+  </si>
+  <si>
+    <t>CNJ02_1_177</t>
+  </si>
+  <si>
+    <t>CNJ02_1_181</t>
+  </si>
+  <si>
+    <t>CNJ02_1_182</t>
+  </si>
+  <si>
+    <t>CNJ02_1_186</t>
+  </si>
+  <si>
+    <t>CNJ02_1_187</t>
+  </si>
+  <si>
+    <t>CNJ02_1_188</t>
+  </si>
+  <si>
+    <t>CNJ02_1_189</t>
+  </si>
+  <si>
+    <t>CNJ02_1_191</t>
+  </si>
+  <si>
+    <t>CNJ02_1_193</t>
+  </si>
+  <si>
+    <t>CNJ02_1_198</t>
+  </si>
+  <si>
+    <t>CNJ02_1_200</t>
+  </si>
+  <si>
+    <t>CNJ02_1_201</t>
+  </si>
+  <si>
+    <t>CNJ02_1_203</t>
+  </si>
+  <si>
+    <t>CNJ02_1_204</t>
+  </si>
+  <si>
+    <t>CNJ02_1_207</t>
+  </si>
+  <si>
+    <t>CNJ02_1_225</t>
+  </si>
+  <si>
+    <t>CNJ02_1_226</t>
+  </si>
+  <si>
+    <t>CNJ02_1_228</t>
+  </si>
+  <si>
+    <t>CNJ02_1_235</t>
   </si>
 </sst>
 </file>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C137" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,13 +1202,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1230,7 +1230,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1252,7 +1252,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1263,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1274,7 +1274,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1285,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1296,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1307,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1318,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1329,7 +1329,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1340,7 +1340,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1351,7 +1351,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1362,7 +1362,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1373,7 +1373,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1384,7 +1384,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1395,7 +1395,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1406,7 +1406,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1417,7 +1417,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1428,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1439,7 +1439,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1450,7 +1450,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1461,7 +1461,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1472,7 +1472,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1483,7 +1483,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1494,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1505,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1516,7 +1516,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1527,7 +1527,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1538,7 +1538,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1549,7 +1549,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1560,7 +1560,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1571,7 +1571,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1582,7 +1582,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1593,7 +1593,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1604,7 +1604,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1626,7 +1626,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1637,7 +1637,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1648,7 +1648,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1659,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1670,7 +1670,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1681,7 +1681,7 @@
         <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1692,7 +1692,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1703,7 +1703,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1714,7 +1714,7 @@
         <v>10</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1725,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1736,7 +1736,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1747,7 +1747,7 @@
         <v>13</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1758,7 +1758,7 @@
         <v>14</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1769,7 +1769,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1780,7 +1780,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1791,7 +1791,7 @@
         <v>17</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1802,7 +1802,7 @@
         <v>18</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1813,7 +1813,7 @@
         <v>19</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1824,7 +1824,7 @@
         <v>20</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1835,7 +1835,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1846,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1857,7 +1857,7 @@
         <v>23</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1868,7 +1868,7 @@
         <v>24</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1879,7 +1879,7 @@
         <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1890,7 +1890,7 @@
         <v>26</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1901,7 +1901,7 @@
         <v>27</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1912,7 +1912,7 @@
         <v>28</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1923,7 +1923,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1934,7 +1934,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1945,7 +1945,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1956,7 +1956,7 @@
         <v>32</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1967,7 +1967,7 @@
         <v>33</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1978,7 +1978,7 @@
         <v>34</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1989,7 +1989,7 @@
         <v>35</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2000,7 +2000,7 @@
         <v>36</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2011,7 +2011,7 @@
         <v>28</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2022,7 +2022,7 @@
         <v>29</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2033,7 +2033,7 @@
         <v>43</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>256</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2044,7 +2044,7 @@
         <v>45</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2055,7 +2055,7 @@
         <v>46</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2066,7 +2066,7 @@
         <v>47</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2077,7 +2077,7 @@
         <v>48</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2088,7 +2088,7 @@
         <v>49</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2099,7 +2099,7 @@
         <v>50</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2110,7 +2110,7 @@
         <v>51</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2121,7 +2121,7 @@
         <v>52</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2132,7 +2132,7 @@
         <v>53</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2143,7 +2143,7 @@
         <v>54</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2165,7 +2165,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2176,7 +2176,7 @@
         <v>3</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2187,7 +2187,7 @@
         <v>4</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2198,7 +2198,7 @@
         <v>5</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2209,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2220,7 +2220,7 @@
         <v>7</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2231,7 +2231,7 @@
         <v>8</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2242,7 +2242,7 @@
         <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2253,7 +2253,7 @@
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2264,7 +2264,7 @@
         <v>11</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2275,7 +2275,7 @@
         <v>12</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2286,7 +2286,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2297,7 +2297,7 @@
         <v>14</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2308,7 +2308,7 @@
         <v>15</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2319,7 +2319,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2330,7 +2330,7 @@
         <v>17</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2341,7 +2341,7 @@
         <v>18</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2352,7 +2352,7 @@
         <v>19</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2363,7 +2363,7 @@
         <v>20</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2374,7 +2374,7 @@
         <v>21</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2385,7 +2385,7 @@
         <v>22</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2396,7 +2396,7 @@
         <v>23</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2407,7 +2407,7 @@
         <v>24</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2418,7 +2418,7 @@
         <v>25</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2429,7 +2429,7 @@
         <v>26</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2440,7 +2440,7 @@
         <v>27</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2451,7 +2451,7 @@
         <v>28</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2462,7 +2462,7 @@
         <v>29</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2473,7 +2473,7 @@
         <v>30</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2484,7 +2484,7 @@
         <v>31</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2495,7 +2495,7 @@
         <v>32</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2506,7 +2506,7 @@
         <v>33</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2517,7 +2517,7 @@
         <v>34</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2528,7 +2528,7 @@
         <v>35</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2539,7 +2539,7 @@
         <v>36</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2550,7 +2550,7 @@
         <v>37</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2561,7 +2561,7 @@
         <v>38</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2572,7 +2572,7 @@
         <v>39</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2583,7 +2583,7 @@
         <v>40</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2594,7 +2594,7 @@
         <v>41</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2605,7 +2605,7 @@
         <v>42</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2616,7 +2616,7 @@
         <v>43</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2627,7 +2627,7 @@
         <v>44</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2638,7 +2638,7 @@
         <v>45</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2649,7 +2649,7 @@
         <v>46</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2660,7 +2660,7 @@
         <v>47</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2671,7 +2671,7 @@
         <v>48</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2682,7 +2682,7 @@
         <v>49</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2693,7 +2693,7 @@
         <v>50</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -2704,7 +2704,7 @@
         <v>51</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2715,7 +2715,7 @@
         <v>52</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2726,7 +2726,7 @@
         <v>53</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2737,7 +2737,7 @@
         <v>54</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -2748,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -2759,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2770,7 +2770,7 @@
         <v>3</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -2781,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -2792,7 +2792,7 @@
         <v>5</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2814,7 +2814,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2825,7 +2825,7 @@
         <v>8</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -2836,7 +2836,7 @@
         <v>9</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -2847,7 +2847,7 @@
         <v>10</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -2858,7 +2858,7 @@
         <v>11</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -2869,7 +2869,7 @@
         <v>12</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -2880,7 +2880,7 @@
         <v>13</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2891,7 +2891,7 @@
         <v>14</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2902,7 +2902,7 @@
         <v>15</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2913,7 +2913,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2924,7 +2924,7 @@
         <v>17</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2935,7 +2935,7 @@
         <v>18</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2946,7 +2946,7 @@
         <v>19</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2957,7 +2957,7 @@
         <v>20</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2968,7 +2968,7 @@
         <v>21</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2979,7 +2979,7 @@
         <v>22</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2990,7 +2990,7 @@
         <v>23</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3001,7 +3001,7 @@
         <v>24</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3012,7 +3012,7 @@
         <v>25</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3023,7 +3023,7 @@
         <v>26</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3034,7 +3034,7 @@
         <v>27</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3045,7 +3045,7 @@
         <v>28</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3056,7 +3056,7 @@
         <v>29</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3067,7 +3067,7 @@
         <v>30</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3078,7 +3078,7 @@
         <v>31</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3089,7 +3089,7 @@
         <v>32</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3100,7 +3100,7 @@
         <v>33</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3111,7 +3111,7 @@
         <v>34</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3122,7 +3122,7 @@
         <v>35</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3133,7 +3133,7 @@
         <v>36</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3144,7 +3144,7 @@
         <v>37</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3155,7 +3155,7 @@
         <v>38</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3166,7 +3166,7 @@
         <v>39</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3177,7 +3177,7 @@
         <v>40</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3188,7 +3188,7 @@
         <v>41</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3199,7 +3199,7 @@
         <v>42</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3210,7 +3210,7 @@
         <v>43</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3221,7 +3221,7 @@
         <v>44</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3232,7 +3232,7 @@
         <v>45</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3243,7 +3243,7 @@
         <v>46</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3254,7 +3254,7 @@
         <v>47</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3265,7 +3265,7 @@
         <v>48</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3276,7 +3276,7 @@
         <v>49</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3287,7 +3287,7 @@
         <v>50</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3298,7 +3298,7 @@
         <v>51</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3309,7 +3309,7 @@
         <v>52</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3320,7 +3320,7 @@
         <v>53</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3331,7 +3331,7 @@
         <v>54</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -3342,7 +3342,7 @@
         <v>2</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -3353,7 +3353,7 @@
         <v>3</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3364,7 +3364,7 @@
         <v>4</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3375,7 +3375,7 @@
         <v>5</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -3386,7 +3386,7 @@
         <v>6</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -3397,7 +3397,7 @@
         <v>7</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -3408,7 +3408,7 @@
         <v>8</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -3419,7 +3419,7 @@
         <v>9</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -3430,7 +3430,7 @@
         <v>10</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -3441,7 +3441,7 @@
         <v>11</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -3452,7 +3452,7 @@
         <v>12</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -3463,7 +3463,7 @@
         <v>13</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -3474,7 +3474,7 @@
         <v>14</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3485,7 +3485,7 @@
         <v>15</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -3496,7 +3496,7 @@
         <v>16</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -3507,7 +3507,7 @@
         <v>17</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -3518,7 +3518,7 @@
         <v>18</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3529,7 +3529,7 @@
         <v>19</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -3540,7 +3540,7 @@
         <v>20</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -3551,7 +3551,7 @@
         <v>21</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3562,7 +3562,7 @@
         <v>22</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -3573,7 +3573,7 @@
         <v>23</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -3584,7 +3584,7 @@
         <v>24</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -3595,7 +3595,7 @@
         <v>25</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -3606,7 +3606,7 @@
         <v>26</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -3617,7 +3617,7 @@
         <v>27</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -3628,7 +3628,7 @@
         <v>28</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -3639,7 +3639,7 @@
         <v>29</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -3650,7 +3650,7 @@
         <v>30</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -3661,7 +3661,7 @@
         <v>31</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -3672,7 +3672,7 @@
         <v>32</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -3683,7 +3683,7 @@
         <v>33</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -3694,7 +3694,7 @@
         <v>34</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -3705,7 +3705,7 @@
         <v>35</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -3716,7 +3716,7 @@
         <v>36</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -3727,7 +3727,7 @@
         <v>37</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -3738,7 +3738,7 @@
         <v>38</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -3749,7 +3749,7 @@
         <v>39</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -3760,7 +3760,7 @@
         <v>40</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -3771,7 +3771,7 @@
         <v>41</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -3782,7 +3782,7 @@
         <v>15</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -3793,7 +3793,7 @@
         <v>19</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -3804,7 +3804,7 @@
         <v>20</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -3815,7 +3815,7 @@
         <v>25</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -3826,7 +3826,7 @@
         <v>29</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -3837,7 +3837,7 @@
         <v>30</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -3848,7 +3848,7 @@
         <v>34</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -3859,7 +3859,7 @@
         <v>35</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -3870,7 +3870,7 @@
         <v>36</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -3881,7 +3881,7 @@
         <v>37</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -3892,7 +3892,7 @@
         <v>39</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -3903,7 +3903,7 @@
         <v>41</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -3914,7 +3914,7 @@
         <v>46</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -3925,7 +3925,7 @@
         <v>48</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -3936,7 +3936,7 @@
         <v>49</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -3947,7 +3947,7 @@
         <v>51</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3958,7 +3958,7 @@
         <v>52</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3969,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3980,7 +3980,7 @@
         <v>19</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3991,7 +3991,7 @@
         <v>20</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -4002,7 +4002,7 @@
         <v>22</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -4013,7 +4013,7 @@
         <v>29</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>